<commit_message>
changes on mld & add database tables
</commit_message>
<xml_diff>
--- a/MLD.xlsx
+++ b/MLD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\DESKTOP-JTM1HD6\Projet_Dev_Web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A9DB04-8808-42B1-A710-4BBF2449E45B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B5B823-5AB1-4298-91F6-6E614C7D94BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9055CE3F-A7A5-4744-A32A-9E1E71536FE4}"/>
+    <workbookView xWindow="7995" yWindow="1785" windowWidth="21600" windowHeight="11385" xr2:uid="{9055CE3F-A7A5-4744-A32A-9E1E71536FE4}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="31">
   <si>
     <t>User</t>
   </si>
@@ -116,10 +116,16 @@
     <t>UserID_2</t>
   </si>
   <si>
-    <t>Login</t>
-  </si>
-  <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>MessageID</t>
+  </si>
+  <si>
+    <t>Text</t>
   </si>
 </sst>
 </file>
@@ -252,9 +258,18 @@
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -264,19 +279,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,9 +522,9 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>11206</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -534,8 +540,61 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2274794" y="3496235"/>
-          <a:ext cx="2308412" cy="1344706"/>
+          <a:off x="2274794" y="6555441"/>
+          <a:ext cx="11206" cy="963706"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>757518</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>6724</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>6724</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>17930</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Connecteur droit avec flèche 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1400287-1548-4AED-9DF9-ED58339B524B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1519518" y="7918077"/>
+          <a:ext cx="11206" cy="963706"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -861,257 +920,262 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{049006A2-EEB0-434F-84A3-E5C5AEFD4F61}">
-  <dimension ref="B3:N43"/>
+  <dimension ref="A3:N50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>9</v>
-      </c>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F17" s="1"/>
     </row>
-    <row r="19" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="15"/>
+      <c r="D19" s="16"/>
+    </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="5"/>
-      <c r="G20" s="3" t="s">
+      <c r="B20" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="H20" s="4"/>
-      <c r="I20" s="5"/>
-      <c r="L20" s="3" t="s">
+      <c r="H20" s="15"/>
+      <c r="I20" s="16"/>
+      <c r="L20" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="M20" s="4"/>
-      <c r="N20" s="5"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="16"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B21" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21" s="13" t="s">
+      <c r="B21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H21" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="H21" s="13" t="s">
+      <c r="I21" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="L21" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M21" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="I21" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="L21" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="M21" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="N21" s="14" t="s">
+      <c r="N21" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B22" s="6" t="s">
-        <v>2</v>
+      <c r="B22" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G22" s="6" t="s">
+      <c r="D22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="2" t="s">
         <v>1</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I22" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="L22" s="6" t="s">
+      <c r="I22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L22" s="2" t="s">
         <v>8</v>
       </c>
       <c r="M22" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="N22" s="7" t="s">
+      <c r="N22" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="23" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="6" t="s">
-        <v>3</v>
+      <c r="B23" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G23" s="6" t="s">
+      <c r="D23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I23" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="L23" s="8" t="s">
+      <c r="I23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="L23" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="M23" s="9" t="s">
+      <c r="M23" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="N23" s="10" t="s">
+      <c r="N23" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B24" s="6" t="s">
-        <v>4</v>
+      <c r="B24" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G24" s="6" t="s">
+      <c r="D24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>12</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I24" s="7" t="s">
+      <c r="I24" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="25" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" s="9" t="s">
+      <c r="B25" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D25" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G25" s="6" t="s">
+      <c r="D25" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G25" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I25" s="7" t="s">
+      <c r="I25" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="G26" s="6" t="s">
+      <c r="G26" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I26" s="7" t="s">
+      <c r="I26" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="27" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G27" s="8" t="s">
+      <c r="G27" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H27" s="9" t="s">
+      <c r="H27" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I27" s="10" t="s">
+      <c r="I27" s="6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="30" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="5"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="16"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B32" s="12" t="s">
+      <c r="B32" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="D32" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="12" t="s">
+      <c r="B33" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D33" s="14" t="s">
+      <c r="D33" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="34" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="16" t="s">
+      <c r="C34" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D34" s="17" t="s">
-        <v>9</v>
-      </c>
-    </row>
+      <c r="D34" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D40" s="1"/>
+      <c r="B40" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C40" s="15"/>
+      <c r="D40" s="16"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
@@ -1119,34 +1183,67 @@
       <c r="I40" s="1"/>
     </row>
     <row r="41" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>9</v>
+      </c>
       <c r="E41" s="1"/>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F42" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G42" s="4"/>
-      <c r="H42" s="5"/>
-    </row>
-    <row r="43" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F43" s="15" t="s">
+    <row r="46" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B47" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C47" s="15"/>
+      <c r="D47" s="16"/>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B48" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G43" s="16" t="s">
+      <c r="C49" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H43" s="17" t="s">
+      <c r="D49" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D50" s="6" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B20:D20"/>
+  <mergeCells count="7">
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B19:D19"/>
     <mergeCell ref="G20:I20"/>
     <mergeCell ref="L20:N20"/>
-    <mergeCell ref="F42:H42"/>
+    <mergeCell ref="B40:D40"/>
     <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B4:D4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
ajout du powerpoint de presentation
</commit_message>
<xml_diff>
--- a/MLD.xlsx
+++ b/MLD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\DESKTOP-JTM1HD6\Projet_Dev_Web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B5B823-5AB1-4298-91F6-6E614C7D94BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{241FEDBC-F3BA-4F11-852D-DA84138DF9A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7995" yWindow="1785" windowWidth="21600" windowHeight="11385" xr2:uid="{9055CE3F-A7A5-4744-A32A-9E1E71536FE4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9055CE3F-A7A5-4744-A32A-9E1E71536FE4}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -270,6 +270,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -279,10 +283,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -569,16 +569,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>757518</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>13607</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>6724</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>6724</xdr:colOff>
+      <xdr:colOff>13607</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>17930</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -592,9 +592,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1519518" y="7918077"/>
-          <a:ext cx="11206" cy="963706"/>
+        <a:xfrm flipV="1">
+          <a:off x="1537607" y="7932965"/>
+          <a:ext cx="0" cy="966106"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -922,8 +922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{049006A2-EEB0-434F-84A3-E5C5AEFD4F61}">
   <dimension ref="A3:N50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AF45" sqref="AF45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -932,9 +932,9 @@
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
@@ -943,7 +943,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="18"/>
+      <c r="B9" s="14"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
@@ -952,11 +952,11 @@
     </row>
     <row r="18" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="16"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="18"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
@@ -968,16 +968,16 @@
       <c r="D20" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="H20" s="15"/>
-      <c r="I20" s="16"/>
-      <c r="L20" s="14" t="s">
+      <c r="H20" s="17"/>
+      <c r="I20" s="18"/>
+      <c r="L20" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="M20" s="15"/>
-      <c r="N20" s="16"/>
+      <c r="M20" s="17"/>
+      <c r="N20" s="18"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
@@ -1130,11 +1130,11 @@
     </row>
     <row r="30" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B31" s="14" t="s">
+      <c r="B31" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="15"/>
-      <c r="D31" s="16"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="18"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B32" s="7" t="s">
@@ -1171,11 +1171,11 @@
     </row>
     <row r="39" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B40" s="14" t="s">
+      <c r="B40" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C40" s="15"/>
-      <c r="D40" s="16"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="18"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
@@ -1196,11 +1196,11 @@
     </row>
     <row r="46" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="47" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B47" s="14" t="s">
+      <c r="B47" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C47" s="15"/>
-      <c r="D47" s="16"/>
+      <c r="C47" s="17"/>
+      <c r="D47" s="18"/>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48" s="7" t="s">

</xml_diff>